<commit_message>
WIP - bucketwise data
</commit_message>
<xml_diff>
--- a/data/trends.xlsx
+++ b/data/trends.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="91">
   <si>
     <t>date</t>
   </si>
@@ -270,6 +271,21 @@
   <si>
     <t>English Premier League</t>
   </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Politics</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Elections</t>
+  </si>
 </sst>
 </file>
 
@@ -308,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -324,6 +340,9 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -333,6 +352,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -14237,4 +14260,702 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="28.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>